<commit_message>
created parallel or multi-thread request resulting scraping multiple pages at a time
</commit_message>
<xml_diff>
--- a/myntra_bra_links.xlsx
+++ b/myntra_bra_links.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,82 +463,98 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.myntra.com/bra/wacoal/wacoal-bra-full-coverage-underwired/35327512/buy</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+          <t>https://www.myntra.com/bra/amante/amante-solid-padded-wired-multiway-strapless-bra---bra10808/2528934/buy</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Amante</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Solid Padded Wired Multiway Strapless Bra - BRA10808</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>663 Ratings</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.myntra.com/bra/triumph/triumph-pink-wireless-big-cup-high-support-minimizer-bra/18185210/buy</t>
+          <t>https://www.myntra.com/bra/marks+%26+spencer/marks--spencer-bra-full-coverage-underwired-lightly-padded/32878492/buy</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Triumph</t>
+          <t>Marks &amp; Spencer</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pink Wireless Big-Cup High Support Minimizer Bra</t>
+          <t>Bra Full Coverage Underwired Lightly Padded</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>143 Ratings</t>
+          <t>33 Ratings</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.myntra.com/bra/you+got+plan+b/you-got-plan-b-cotton-elastane-pack-of-3-girl-basic-sports-full-coverage-bra/30309097/buy</t>
+          <t>https://www.myntra.com/bra/amante/amante-floral-bra-full-coverage/28111984/buy</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>You Got Plan B</t>
+          <t>Amante</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Cotton Elastane Pack of 3 Girl Basic Sports Full Coverage Bra</t>
+          <t>Floral Bra Full Coverage</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>44 Ratings</t>
+          <t>357 Ratings</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.myntra.com/bra/dchica/girls-pack-of-4-double-layer-premium-cotton-non-wired-non-padded-beginners-bra-dcbrdc6444xxxs/13272998/buy</t>
+          <t>https://www.myntra.com/bra/amante/amante-floral-bra-full-coverage/28111990/buy</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DChica</t>
+          <t>Amante</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Girls Pack Of 4 Double Layer Premium Cotton Non-Wired Non Padded Beginners Bra DCBRDC6444/xxxs</t>
+          <t>Floral Bra Full Coverage</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -548,180 +564,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>548 Ratings</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>https://www.myntra.com/bra/triumph/triumph-minimizer-21-wired-non-padded-comfortable-high-support-big-cup-bra/363038/buy</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Triumph</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Minimizer 21 Wired Non Padded Comfortable High Support Big-Cup Bra</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>4.6</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1.5k Ratings</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>https://www.myntra.com/bra/braafee/girls-beginners-non-padded-teenager-full-coverage-cotton-bra/35227041/buy</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>https://www.myntra.com/bra/dressberry/dressberry-beige-solid-non-wired-lightly-padded-everyday-bra-db-cam-pad-01d/9050725/buy</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>DressBerry</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Beige Solid Non-Wired Lightly Padded Everyday Bra DB-CAM-PAD-01D</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>4.5</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>36.9k Ratings</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>https://www.myntra.com/bra/triumph/triumph-minimizer-21-wireless-non-padded-comfortable-high-support-big-cup-bra/363026/buy</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Triumph</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Minimizer 21 Wireless Non Padded Comfortable High Support Big-Cup Bra</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>4.6</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1.3k Ratings</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>https://www.myntra.com/bra/sillysally/sillysally-girls-pack-of-3-full-coverage-removable-padded-beginners-bra---all-day-comfort/28173750/buy</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Sillysally</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Girls Pack of 3 Full Coverage Removable Padded Beginners Bra - All Day Comfort</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>4.2</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>28 Ratings</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>https://www.myntra.com/bra/dchica/dchica-girls-pack-of-4-non-padded-full-coverage-all-day-comfort-seamless-cotton-sports-bra/22790858/buy</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>DChica</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Girls Pack Of 4 Non-Padded Full Coverage All Day Comfort Seamless Cotton Sports Bra</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>4.5</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>107 Ratings</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>https://www.myntra.com/bra/triumph/triumph-doreen-wireless-non-padded-full-coverage-support-big-cup-classics-bra/149663/buy</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Triumph</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Doreen Wireless Non Padded Full Coverage Support Big-Cup Classics Bra</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>4.6</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>336 Ratings</t>
+          <t>623 Ratings</t>
         </is>
       </c>
     </row>

</xml_diff>